<commit_message>
Update profiles descriptions 5a7b499f8a45d47fef5290858c2e29f407b199f4
</commit_message>
<xml_diff>
--- a/feature/harmonize-profiles-descriptions/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/feature/harmonize-profiles-descriptions/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-03T16:53:35+00:00</t>
+    <t>2024-12-03T17:09:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil de Bundle qui représente le flux de réponse contenant les créneaux disponibles dans le cadre du service d'agrégation de créneaux de la plateforme SAS (Service d'accès aux soins)</t>
+    <t>Profil de Bundle qui représente le flux de réponse contenant les créneaux disponibles dans le cadre du service d'agrégation de créneaux de la plateforme SAS - Cas d'usage PS Indiv</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>